<commit_message>
default testing block mastery criterion update
</commit_message>
<xml_diff>
--- a/stimuli, instructions and parameters.xlsx
+++ b/stimuli, instructions and parameters.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26819"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26929"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="sheet 1" sheetId="3" r:id="rId1"/>
@@ -2018,7 +2018,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2119,7 +2119,7 @@
         <v>8</v>
       </c>
       <c r="J2" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K2" s="2">
         <v>10</v>

</xml_diff>

<commit_message>
updated docs and default settings in line
</commit_message>
<xml_diff>
--- a/stimuli, instructions and parameters.xlsx
+++ b/stimuli, instructions and parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26929"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="sheet 1" sheetId="3" r:id="rId1"/>
@@ -2018,7 +2018,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2110,25 +2110,25 @@
         <v>11</v>
       </c>
       <c r="G2" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
       </c>
       <c r="I2" s="5">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="J2" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K2" s="2">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="L2" s="2">
         <v>1</v>
       </c>
       <c r="M2" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>28</v>

</xml_diff>